<commit_message>
Edit Projektplanung und Pflichtenheft
</commit_message>
<xml_diff>
--- a/docu/Projektplanung.xlsx
+++ b/docu/Projektplanung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11592"/>
   </bookViews>
   <sheets>
     <sheet name="Projekt" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -597,28 +597,31 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>17</xdr:col>
-          <xdr:colOff>200025</xdr:colOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:rowOff>259080</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Drehfeld 5" hidden="1">
+            <xdr:cNvPr id="1029" name="Drehfeld 5" descr="Period Highlight Spin Control" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -626,6 +629,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -869,23 +878,23 @@
   <dimension ref="B2:BQ14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
-    <col min="2" max="2" width="21.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7.25" style="7" customWidth="1"/>
-    <col min="8" max="8" width="4.25" style="1" customWidth="1"/>
-    <col min="9" max="28" width="2.75" style="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="4.21875" style="1" customWidth="1"/>
+    <col min="9" max="28" width="2.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:69" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:69" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -895,7 +904,7 @@
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:69" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -944,7 +953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -957,12 +966,12 @@
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:69" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:69" x14ac:dyDescent="0.35">
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:69" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:69" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
         <v>3</v>
@@ -986,7 +995,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:69" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1020,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1201,7 +1210,7 @@
       </c>
       <c r="BQ8" s="1"/>
     </row>
-    <row r="9" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="14" t="s">
         <v>15</v>
       </c>
@@ -1211,79 +1220,115 @@
       <c r="D9" s="15">
         <v>3</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>3</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10" s="15">
         <v>3</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="E10" s="15">
+        <v>4</v>
+      </c>
+      <c r="F10" s="15">
+        <v>3</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" s="15">
         <v>1</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
+      <c r="E11" s="15">
+        <v>7</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" s="15">
         <v>4</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="15">
+        <v>8</v>
+      </c>
+      <c r="F12" s="15">
+        <v>4</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13" s="15">
         <v>2</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="E13" s="15">
+        <v>12</v>
+      </c>
+      <c r="F13" s="15">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:69" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="15">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D14" s="15">
         <v>2</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
+      <c r="E14" s="15">
+        <v>14</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1339,15 +1384,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>68580</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>30480</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>200025</xdr:colOff>
+                    <xdr:colOff>198120</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>257175</xdr:rowOff>
+                    <xdr:rowOff>259080</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>